<commit_message>
Domain entity and Dto folder
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Miss.AliZadeh" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="48">
   <si>
     <t>Attributes</t>
   </si>
@@ -154,6 +154,24 @@
   <si>
     <t>DTo{ProducId = Int , 
 UnitPrice = int  }</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>List&lt;categoryt&gt;</t>
+  </si>
+  <si>
+    <t>GetActiveChildCategory</t>
+  </si>
+  <si>
+    <t>GetActiveList</t>
+  </si>
+  <si>
+    <t>GetInActiveChildCategory</t>
+  </si>
+  <si>
+    <t>GetInActiveList</t>
   </si>
 </sst>
 </file>
@@ -265,10 +283,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -553,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView rightToLeft="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -782,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -815,7 +833,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -838,7 +856,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -859,7 +877,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
@@ -880,7 +898,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
@@ -901,7 +919,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
@@ -922,7 +940,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
         <v>27</v>
       </c>
@@ -943,7 +961,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
@@ -964,7 +982,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="5" t="s">
         <v>29</v>
       </c>
@@ -985,7 +1003,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1006,7 +1024,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1027,7 +1045,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
@@ -1048,7 +1066,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1069,7 +1087,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1084,7 +1102,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1110,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1161,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1166,10 +1184,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
@@ -1181,10 +1205,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
@@ -1196,10 +1226,16 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>39</v>
       </c>
@@ -1211,10 +1247,16 @@
       </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>39</v>
       </c>
@@ -1226,10 +1268,16 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>39</v>
       </c>
@@ -1241,10 +1289,16 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E8" s="6" t="s">
         <v>39</v>
       </c>
@@ -1256,10 +1310,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>39</v>
       </c>
@@ -1271,7 +1331,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1286,7 +1346,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1301,7 +1361,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>

</xml_diff>